<commit_message>
Fix nomor aju sync logic in entitas sheet
</commit_message>
<xml_diff>
--- a/data/templates/PIB_TEMPLATE.xlsx
+++ b/data/templates/PIB_TEMPLATE.xlsx
@@ -1,39 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10110"/>
+  <workbookPr defaultThemeVersion="202300"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anilpal/Documents/Inabata_Production/data/templates/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E8BF0A6-1877-AB4C-B9FB-1A1F2E35ABC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="33600" windowHeight="20400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="HEADER" r:id="rId3" sheetId="1"/>
-    <sheet name="ENTITAS" r:id="rId4" sheetId="2"/>
-    <sheet name="DOKUMEN" r:id="rId5" sheetId="3"/>
-    <sheet name="PENGANGKUT" r:id="rId6" sheetId="4"/>
-    <sheet name="KEMASAN" r:id="rId7" sheetId="5"/>
-    <sheet name="KONTAINER" r:id="rId8" sheetId="6"/>
-    <sheet name="KOMPONENBIAYA" r:id="rId9" sheetId="7"/>
-    <sheet name="BARANG" r:id="rId10" sheetId="8"/>
-    <sheet name="BARANGTARIF" r:id="rId11" sheetId="9"/>
-    <sheet name="BARANGDOKUMEN" r:id="rId12" sheetId="10"/>
-    <sheet name="BARANGENTITAS" r:id="rId13" sheetId="11"/>
-    <sheet name="BARANGSPEKKHUSUS" r:id="rId14" sheetId="12"/>
-    <sheet name="BARANGVD" r:id="rId15" sheetId="13"/>
-    <sheet name="BAHANBAKU" r:id="rId16" sheetId="14"/>
-    <sheet name="BAHANBAKUTARIF" r:id="rId17" sheetId="15"/>
-    <sheet name="BAHANBAKUDOKUMEN" r:id="rId18" sheetId="16"/>
-    <sheet name="PUNGUTAN" r:id="rId19" sheetId="17"/>
-    <sheet name="JAMINAN" r:id="rId20" sheetId="18"/>
-    <sheet name="BANKDEVISA" r:id="rId21" sheetId="19"/>
-    <sheet name="VERSI" r:id="rId22" sheetId="20"/>
-    <sheet name="RESPON" r:id="rId23" sheetId="21"/>
+    <sheet name="HEADER" sheetId="1" r:id="rId1"/>
+    <sheet name="ENTITAS" sheetId="2" r:id="rId2"/>
+    <sheet name="DOKUMEN" sheetId="3" r:id="rId3"/>
+    <sheet name="PENGANGKUT" sheetId="4" r:id="rId4"/>
+    <sheet name="KEMASAN" sheetId="5" r:id="rId5"/>
+    <sheet name="KONTAINER" sheetId="6" r:id="rId6"/>
+    <sheet name="KOMPONENBIAYA" sheetId="7" r:id="rId7"/>
+    <sheet name="BARANG" sheetId="8" r:id="rId8"/>
+    <sheet name="BARANGTARIF" sheetId="9" r:id="rId9"/>
+    <sheet name="BARANGDOKUMEN" sheetId="10" r:id="rId10"/>
+    <sheet name="BARANGENTITAS" sheetId="11" r:id="rId11"/>
+    <sheet name="BARANGSPEKKHUSUS" sheetId="12" r:id="rId12"/>
+    <sheet name="BARANGVD" sheetId="13" r:id="rId13"/>
+    <sheet name="BAHANBAKU" sheetId="14" r:id="rId14"/>
+    <sheet name="BAHANBAKUTARIF" sheetId="15" r:id="rId15"/>
+    <sheet name="BAHANBAKUDOKUMEN" sheetId="16" r:id="rId16"/>
+    <sheet name="PUNGUTAN" sheetId="17" r:id="rId17"/>
+    <sheet name="JAMINAN" sheetId="18" r:id="rId18"/>
+    <sheet name="BANKDEVISA" sheetId="19" r:id="rId19"/>
+    <sheet name="VERSI" sheetId="20" r:id="rId20"/>
+    <sheet name="RESPON" sheetId="21" r:id="rId21"/>
   </sheets>
-  <definedNames/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="250">
   <si>
     <t>NOMOR AJU</t>
   </si>
@@ -345,9 +352,6 @@
   </si>
   <si>
     <t>FLAG PROPORSIONAL NETTO</t>
-  </si>
-  <si>
-    <t>00002701069420251230006876</t>
   </si>
   <si>
     <t>27</t>
@@ -791,21 +795,22 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd-MM-yyyy HH:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11.00"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="12.00"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -830,125 +835,442 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="0E2841"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E8E8E8"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="156082"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="E97132"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="196B24"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="0F9ED5"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="A02B93"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="4EA72E"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="467886"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="96607D"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false" autoPageBreaks="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:DC2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="20.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="20.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="19.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="19.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="18.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="15.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="15.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="20.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="22.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="23.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="16.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="17" max="17" width="16.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="18" max="18" width="24.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="19" max="19" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="19.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="22.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="21.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="24.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="25.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="25.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="18.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="14.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="32" max="32" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="33" max="33" width="19.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="34" max="34" width="19.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="35" max="35" width="14.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="36" max="36" width="11.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="14.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="23.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="41" max="41" width="20.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="42" max="42" width="26.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="43" max="43" width="23.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="44" max="44" width="22.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="45" max="45" width="22.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="46" max="46" width="9.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="47" max="47" width="18.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="48" max="48" width="15.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="49" max="49" width="14.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="50" max="50" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="51" max="51" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="52" max="52" width="16.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="53" max="53" width="16.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="54" max="54" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="55" max="55" width="20.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="56" max="56" width="22.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="57" max="57" width="11.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="58" max="58" width="9.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="60" max="60" width="11.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="61" max="61" width="11.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="62" max="62" width="14.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="63" max="63" width="9.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="64" max="64" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="65" max="65" width="15.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="66" max="66" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="67" max="67" width="9.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="70" max="70" width="15.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="71" max="71" width="16.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="74" max="74" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="76" max="76" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="77" max="77" width="22.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="78" max="78" width="11.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="79" max="79" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="83" max="83" width="16.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="84" max="84" width="19.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="85" max="85" width="16.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="86" max="86" width="19.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="87" max="87" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="88" max="88" width="14.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="89" max="89" width="21.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="90" max="90" width="18.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="91" max="91" width="20.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="92" max="92" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="93" max="93" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="94" max="94" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="95" max="95" width="15.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="96" max="96" width="21.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="97" max="97" width="24.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="98" max="98" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="99" max="99" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="100" max="100" width="16.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="101" max="101" width="18.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="102" max="102" width="22.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="103" max="103" width="23.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="104" max="104" width="15.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="105" max="105" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="106" max="106" width="24.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="107" max="107" width="24.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="44" max="45" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="50" max="51" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="52" max="53" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="85" max="85" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="86" max="86" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="91" max="91" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="92" max="93" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="94" max="94" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="97" max="97" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="101" max="101" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="104" max="104" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="106" max="107" width="24.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:107" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1271,187 +1593,168 @@
         <v>103</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:107" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
         <v>104</v>
       </c>
-      <c r="B2" t="s">
-        <v>105</v>
-      </c>
-      <c r="BU2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="BV2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="BY2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="CB2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="CT2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="CU2" t="n">
-        <v>0.0</v>
+      <c r="BU2">
+        <v>0</v>
+      </c>
+      <c r="BV2">
+        <v>0</v>
+      </c>
+      <c r="BY2">
+        <v>0</v>
+      </c>
+      <c r="CB2">
+        <v>0</v>
+      </c>
+      <c r="CT2">
+        <v>0</v>
+      </c>
+      <c r="CU2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="0" useFirstPageNumber="false" blackAndWhite="false" orientation="portrait"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false" autoPageBreaks="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="0" useFirstPageNumber="false" blackAndWhite="false" orientation="portrait"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false" autoPageBreaks="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="0" useFirstPageNumber="false" blackAndWhite="false" orientation="portrait"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false" autoPageBreaks="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="0" useFirstPageNumber="false" blackAndWhite="false" orientation="portrait"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false" autoPageBreaks="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="15.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="16.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>61</v>
@@ -1463,125 +1766,120 @@
         <v>67</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="0" useFirstPageNumber="false" blackAndWhite="false" orientation="portrait"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false" autoPageBreaks="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:AO1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="16.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="21.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="14.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="15.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="18.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="17" max="17" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="18" max="18" width="18.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="19" max="19" width="20.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="15.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="11.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="16.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="11.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="33" max="33" width="9.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="34" max="34" width="18.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="35" max="35" width="22.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="36" max="36" width="9.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="16.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="18.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="18.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="41" max="41" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:41" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>77</v>
@@ -1596,306 +1894,290 @@
         <v>69</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>71</v>
       </c>
       <c r="AB1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="AD1" s="1" t="s">
         <v>74</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AG1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="AH1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>196</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="0" useFirstPageNumber="false" blackAndWhite="false" orientation="portrait"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false" autoPageBreaks="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="16.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="21.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="14.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="11.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="15.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="16.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="16.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="21.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="14.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="19.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="20.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="17" max="17" width="24.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="18" max="18" width="9.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="19" max="19" width="15.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="24.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="9.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="15.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="15.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:25" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>217</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="T1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="0" useFirstPageNumber="false" blackAndWhite="false" orientation="portrait"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false" autoPageBreaks="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="16.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="21.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="0" useFirstPageNumber="false" blackAndWhite="false" orientation="portrait"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false" autoPageBreaks="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="21.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="20.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="15.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="0" useFirstPageNumber="false" blackAndWhite="false" orientation="portrait"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false" autoPageBreaks="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="14.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="16.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="14.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="9.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="20.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1903,709 +2185,653 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>227</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="0" useFirstPageNumber="false" blackAndWhite="false" orientation="portrait"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false" autoPageBreaks="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="0" useFirstPageNumber="false" blackAndWhite="false" orientation="portrait"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false" autoPageBreaks="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="21.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="16.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="15.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="15.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="19.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="21.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="14.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="27.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="14.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="P1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
         <v>124</v>
       </c>
+      <c r="C2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" t="s">
+        <v>125</v>
+      </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>104</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D3" t="s">
         <v>125</v>
       </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" t="s">
         <v>125</v>
-      </c>
-      <c r="D2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B3" t="s">
-        <v>127</v>
-      </c>
-      <c r="C3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B4" t="s">
-        <v>128</v>
-      </c>
-      <c r="C4" t="s">
-        <v>128</v>
-      </c>
-      <c r="D4" t="s">
-        <v>126</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="0" useFirstPageNumber="false" blackAndWhite="false" orientation="portrait"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false" autoPageBreaks="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>246</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>247</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="0" useFirstPageNumber="false" blackAndWhite="false" orientation="portrait"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false" autoPageBreaks="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="15.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C1" t="s">
         <v>248</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>249</v>
-      </c>
-      <c r="D1" t="s">
-        <v>250</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="0" useFirstPageNumber="false" blackAndWhite="false" orientation="portrait"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false" autoPageBreaks="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="14.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="16.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="15.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>131</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>132</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="0" useFirstPageNumber="false" blackAndWhite="false" orientation="portrait"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false" autoPageBreaks="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="16.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="16.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="26.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="0" useFirstPageNumber="false" blackAndWhite="false" orientation="portrait"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false" autoPageBreaks="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="15.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>142</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="0" useFirstPageNumber="false" blackAndWhite="false" orientation="portrait"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false" autoPageBreaks="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="15.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="22.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="21.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="20.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>146</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="0" useFirstPageNumber="false" blackAndWhite="false" orientation="portrait"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false" autoPageBreaks="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:T1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="14.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="26.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="9.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="19.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="15.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="9.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="26.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="17" max="17" width="18.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="18" max="18" width="21.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:20" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>239</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>60</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>245</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="0" useFirstPageNumber="false" blackAndWhite="false" orientation="portrait"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false" autoPageBreaks="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:BR1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="14.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="15.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="18.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="18.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="17" max="17" width="20.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="18" max="18" width="15.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="19" max="19" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="11.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="11.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="9.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="32" max="32" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="34" max="34" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="35" max="35" width="16.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="36" max="36" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="37" max="37" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="14.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="11.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="41" max="41" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="42" max="42" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="43" max="43" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="44" max="44" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="45" max="45" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="46" max="46" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="47" max="47" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="48" max="48" width="20.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="49" max="49" width="21.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="50" max="50" width="20.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="51" max="51" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="52" max="52" width="17.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="53" max="53" width="18.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="54" max="54" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="55" max="55" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="56" max="56" width="16.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="57" max="57" width="19.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="58" max="58" width="9.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="59" max="59" width="18.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="60" max="60" width="22.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="61" max="61" width="9.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="62" max="62" width="16.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="63" max="63" width="18.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="64" max="64" width="18.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="65" max="65" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="66" max="66" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="67" max="67" width="18.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="68" max="68" width="23.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="69" max="69" width="30.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="70" max="70" width="26.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="43" max="47" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="51" max="52" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="63" max="64" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="26.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:70" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>77</v>
@@ -2617,19 +2843,19 @@
         <v>78</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="X1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="Y1" s="1" t="s">
-        <v>164</v>
       </c>
       <c r="Z1" s="1" t="s">
         <v>69</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>71</v>
@@ -2644,25 +2870,25 @@
         <v>64</v>
       </c>
       <c r="AF1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="AM1" s="1" t="s">
         <v>61</v>
@@ -2671,202 +2897,194 @@
         <v>74</v>
       </c>
       <c r="AO1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AP1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="AR1" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="AS1" s="1" t="s">
         <v>30</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AU1" s="1" t="s">
         <v>88</v>
       </c>
       <c r="AV1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="AW1" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="BL1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="BN1" s="1" t="s">
-        <v>196</v>
       </c>
       <c r="BO1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="BP1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="BQ1" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="BR1" s="1" t="s">
-        <v>199</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="0" useFirstPageNumber="false" blackAndWhite="false" orientation="portrait"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false" autoPageBreaks="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <sheetPr>
+    <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="14.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="15.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="16.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="16.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="10" max="10" width="21.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="12.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="12" max="12" width="14.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="13" max="13" width="19.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="14" max="14" width="20.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="15" max="15" width="24.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="16" max="16" width="9.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="17" max="17" width="15.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="18" max="18" width="13.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
-    <col min="19" max="19" width="15.42578125" outlineLevel="0" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="R1" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="0" useFirstPageNumber="false" blackAndWhite="false" orientation="portrait"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>